<commit_message>
Add species list to ingrowth form.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/ingrowth/forms/ingrowth/ingrowth.xlsx
+++ b/odk_app/config/tables/ingrowth/forms/ingrowth/ingrowth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joey\Desktop\dev\classes\capstone\app-designer-2.1.6\app\config\tables\ingrowth\forms\ingrowth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\ingrowth\forms\ingrowth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421A5216-4202-4967-8C2C-84AD7BD80995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF709E5-F8C8-4370-BFE8-72996F5495C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="273">
   <si>
     <t>clause</t>
   </si>
@@ -655,6 +655,198 @@
   </si>
   <si>
     <t>select_one_integer</t>
+  </si>
+  <si>
+    <t>ABAM</t>
+  </si>
+  <si>
+    <t>ABCO</t>
+  </si>
+  <si>
+    <t>ABGR</t>
+  </si>
+  <si>
+    <t>ABLA</t>
+  </si>
+  <si>
+    <t>ABMA</t>
+  </si>
+  <si>
+    <t>ABPR</t>
+  </si>
+  <si>
+    <t>ACGL</t>
+  </si>
+  <si>
+    <t>ACMA3</t>
+  </si>
+  <si>
+    <t>ALRU2</t>
+  </si>
+  <si>
+    <t>ALVIS</t>
+  </si>
+  <si>
+    <t>ARME</t>
+  </si>
+  <si>
+    <t>CHCH7</t>
+  </si>
+  <si>
+    <t>CADE27</t>
+  </si>
+  <si>
+    <t>CANO9</t>
+  </si>
+  <si>
+    <t>CONU4</t>
+  </si>
+  <si>
+    <t>FRPU7</t>
+  </si>
+  <si>
+    <t>PICO</t>
+  </si>
+  <si>
+    <t>PIEN</t>
+  </si>
+  <si>
+    <t>PILA</t>
+  </si>
+  <si>
+    <t>PIMO3</t>
+  </si>
+  <si>
+    <t>PIPO</t>
+  </si>
+  <si>
+    <t>PISI</t>
+  </si>
+  <si>
+    <t>POBAT</t>
+  </si>
+  <si>
+    <t>PREM</t>
+  </si>
+  <si>
+    <t>PRUNU</t>
+  </si>
+  <si>
+    <t>PSME</t>
+  </si>
+  <si>
+    <t>QUGA4</t>
+  </si>
+  <si>
+    <t>QUKE</t>
+  </si>
+  <si>
+    <t>TABR2</t>
+  </si>
+  <si>
+    <t>THPL</t>
+  </si>
+  <si>
+    <t>TSHE</t>
+  </si>
+  <si>
+    <t>TSME</t>
+  </si>
+  <si>
+    <t>ABAM - Abies amabilis (Pacific silver fir)</t>
+  </si>
+  <si>
+    <t>ABCO - Abies concolor (white fir)</t>
+  </si>
+  <si>
+    <t>ABGR - Abies grandis (grand fir)</t>
+  </si>
+  <si>
+    <t>ABLA - Abies lasiocarpa (subalpine fir)</t>
+  </si>
+  <si>
+    <t>ABMA - Abies magnifica (Shasta red fir)</t>
+  </si>
+  <si>
+    <t>ABPR - Abies procera (noble fir)</t>
+  </si>
+  <si>
+    <t>ACGL - Acer glabrum (Rocky Mtn maple)</t>
+  </si>
+  <si>
+    <t>ACMA3 - Acer macrophyllum (bigleaf maple)</t>
+  </si>
+  <si>
+    <t>ALRU2 - Alnus rubra (red alder)</t>
+  </si>
+  <si>
+    <t>ALVIS - Alnus viridis ssp sinuata (Sitka alder)</t>
+  </si>
+  <si>
+    <t>ARME - Arbutus menziesii (Pacific madrone)</t>
+  </si>
+  <si>
+    <t>CHCH7 - Chrysolepis chrysophylla (golden chinquapin)</t>
+  </si>
+  <si>
+    <t>CADE27 - Calocedrus decurrens (incense cedar)</t>
+  </si>
+  <si>
+    <t>CANO9 - Callitropsis nootkatensis (Alaska yellow cedar)</t>
+  </si>
+  <si>
+    <t>CONU4 - Cornus nuttalli (Pacific dogwood)</t>
+  </si>
+  <si>
+    <t>FRPU7 - Frangula purshiana (Cascara buckthorn)</t>
+  </si>
+  <si>
+    <t>PICO - Pinus contorta (Lodgepole pine)</t>
+  </si>
+  <si>
+    <t>PIEN - Picea engelmanii (Engelmnn spruce)</t>
+  </si>
+  <si>
+    <t>PILA - Pinus lambertiana (sugar pine)</t>
+  </si>
+  <si>
+    <t>PIMO3 - Pinus monticola (w. white pine)</t>
+  </si>
+  <si>
+    <t>PIPO - Pinus ponderosa (ponderosa pine)</t>
+  </si>
+  <si>
+    <t>PISI - Picea sitchensis (Sitka spruce)</t>
+  </si>
+  <si>
+    <t>POBAT - Populus balsamifer v. trich. (black cottonwood)</t>
+  </si>
+  <si>
+    <t>PREM - Prunus emarginata (bitter cherry)</t>
+  </si>
+  <si>
+    <t>PRUNU - Prunus spp. (cherry)</t>
+  </si>
+  <si>
+    <t>PSME - Pseudotsuga menziesii (Douglas-fir)</t>
+  </si>
+  <si>
+    <t>QUGA4 - Quercus garryana (Oregon white oak)</t>
+  </si>
+  <si>
+    <t>QUKE - Quercus kelloggii (California black oak)</t>
+  </si>
+  <si>
+    <t>TABR2 - Taxus brevifolia (Pacific yew)</t>
+  </si>
+  <si>
+    <t>THPL - Thuja plicata (western redcedar)</t>
+  </si>
+  <si>
+    <t>TSHE - Tsuga heterophylla (western hemlock)</t>
+  </si>
+  <si>
+    <t>TSME - Tsuga mertensiana (mountain hemlock)</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1335,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1397,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D5" t="s">
         <v>82</v>
@@ -1456,17 +1648,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EE1E27-87FD-4841-A3DC-8BD20632DF4F}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2273,6 +2465,359 @@
         <v>206</v>
       </c>
     </row>
+    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>82</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>82</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>82</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>82</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>82</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>82</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>82</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>82</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>82</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>82</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>82</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>82</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>82</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>82</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>82</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>82</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>82</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>82</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>82</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>82</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>82</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>82</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>82</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>82</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>82</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>82</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>82</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
I added basic constraints to all of the survey forms. Also I created a new dircetory called surveyConstraints which contains all the JavaScript constraints which are use in the forms.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/ingrowth/forms/ingrowth/ingrowth.xlsx
+++ b/odk_app/config/tables/ingrowth/forms/ingrowth/ingrowth.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="304">
   <si>
     <t xml:space="preserve">setting_name</t>
   </si>
@@ -106,6 +106,12 @@
     <t xml:space="preserve">display.prompt.text</t>
   </si>
   <si>
+    <t xml:space="preserve">constraint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.contraint_message.text</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin screen</t>
   </si>
   <si>
@@ -124,6 +130,27 @@
     <t xml:space="preserve">Tag</t>
   </si>
   <si>
+    <t xml:space="preserve">(function() { if (data('tag')!=2){return true;} alert('Fix Tag Number'); return false;})()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix Tag Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('tag') == 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tag number already in use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if</t>
+  </si>
+  <si>
     <t xml:space="preserve">select_one_dropdown</t>
   </si>
   <si>
@@ -169,6 +196,84 @@
     <t xml:space="preserve">Crown ratio (%)</t>
   </si>
   <si>
+    <t xml:space="preserve">(function() { if (data('crown_ratio') &lt;= 100  &amp;&amp; data('crown_ratio') &gt;=1){return true;} alert('Crown Ratio Needs to be Fixed'); return false;})()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix Crown Ratio</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">data(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">crown_ratio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) &gt; 100 || data(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'crown_ratio') &lt; 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Crown Ratio must be between 1 and 100</t>
+  </si>
+  <si>
     <t xml:space="preserve">tree_vigor</t>
   </si>
   <si>
@@ -196,19 +301,115 @@
     <t xml:space="preserve">Lean angle (deg)</t>
   </si>
   <si>
+    <t xml:space="preserve">(function() { if (data('lean_angle') &lt;= 120  &amp;&amp; data('lean_angle') &gt;=0){return true;} alert('Lean Angle Needs to be Fixed'); return false;})()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix Lean Angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('lean_angle') &gt; 120 || data('crown_percentage') &lt; 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lean Angle must be between 0 and 120</t>
+  </si>
+  <si>
     <t xml:space="preserve">crown_percentage</t>
   </si>
   <si>
     <t xml:space="preserve">Crown percentage</t>
   </si>
   <si>
+    <t xml:space="preserve">(function() { if (data('crown_percentage') &lt;= 100  &amp;&amp; data('crown_percentage') &gt;=0){return true;} alert('Crown Ratio Needs to be Fixed'); return false;})()</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">data(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">crown_percentage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) &gt; 100 || data(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">'crown_percentage') &lt; 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Crown Percentage must be between 0 and 100</t>
+  </si>
+  <si>
     <t xml:space="preserve">tree_percentage</t>
   </si>
   <si>
     <t xml:space="preserve">Tree percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">note</t>
+    <t xml:space="preserve">(function() { if (data('tree_percentage') &lt;= 100  &amp;&amp; data('tree_percentage') &gt;=0){return true;} alert('Tree Percentage Needs to be Fixed'); return false;})()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix Tree Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('tree_percentage') &gt; 100 || data('tree_percentage') &lt; 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tree Percentage must be between 0 and 100</t>
   </si>
   <si>
     <t xml:space="preserve">Mapping</t>
@@ -226,10 +427,34 @@
     <t xml:space="preserve">Distance (m)</t>
   </si>
   <si>
+    <t xml:space="preserve">(function() { if (data('distance') &lt;= 25.0  &amp;&amp; data('distance') &gt;=0.1){return true;} alert('Distance Needs to be Fixed'); return false;})()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix Distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('distance') &gt; 25 || data('distance') &lt; 0.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance must be between 0.1m and 25.0m</t>
+  </si>
+  <si>
     <t xml:space="preserve">azimuth</t>
   </si>
   <si>
     <t xml:space="preserve">Azimuth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(function() { if (data('azimuth') &lt;= 360  &amp;&amp; data('azimuth') &gt;=0){return true;} alert('Azimuth Range needs to be fixed'); return false;})()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix Azimuth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('azimuth') &gt; 360 || data('azimuth') &lt; 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azimuth value must be between 0 and 360</t>
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
@@ -851,7 +1076,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -874,13 +1099,25 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -932,12 +1169,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1097,7 +1346,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1194,13 +1443,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.71"/>
@@ -1208,10 +1457,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="74.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>22</v>
       </c>
@@ -1230,79 +1481,86 @@
       <c r="F1" s="0" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
-        <v>28</v>
-      </c>
       <c r="E4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="H4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="B5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>44</v>
@@ -1311,197 +1569,476 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="1" t="s">
         <v>50</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="s">
+      <c r="B13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>69</v>
-      </c>
+      <c r="B20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>72</v>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>74</v>
-      </c>
+      <c r="A22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0" t="s">
+      <c r="H23" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="1" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="F27" s="0" t="s">
         <v>80</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1522,7 +2059,7 @@
   </sheetPr>
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1536,10 +2073,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
@@ -1547,1147 +2084,1147 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>112</v>
+        <v>101</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>116</v>
+        <v>101</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>118</v>
+        <v>101</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>120</v>
+        <v>101</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>122</v>
+        <v>101</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>123</v>
+        <v>101</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>125</v>
+        <v>101</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>127</v>
+        <v>101</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>129</v>
+        <v>101</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>131</v>
+        <v>101</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>133</v>
+        <v>101</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>135</v>
+        <v>101</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>137</v>
+        <v>101</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>139</v>
+        <v>101</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>141</v>
+        <v>101</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>142</v>
+        <v>101</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>144</v>
+        <v>101</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>146</v>
+        <v>101</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>148</v>
+        <v>101</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>150</v>
+        <v>101</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>152</v>
+        <v>101</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>154</v>
+        <v>101</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>156</v>
+        <v>101</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>160</v>
+        <v>101</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>162</v>
+        <v>101</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>164</v>
+        <v>101</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>166</v>
+        <v>101</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>168</v>
+        <v>101</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>170</v>
+        <v>101</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>172</v>
+        <v>101</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>174</v>
+        <v>101</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>176</v>
+        <v>101</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>178</v>
+        <v>101</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>180</v>
+        <v>101</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>182</v>
+        <v>101</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>184</v>
+        <v>101</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>186</v>
+        <v>101</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>188</v>
+        <v>101</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>189</v>
+        <v>101</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>191</v>
+        <v>101</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>193</v>
+        <v>101</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>194</v>
+        <v>101</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>196</v>
+        <v>101</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>198</v>
+        <v>101</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>200</v>
+        <v>101</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>202</v>
+        <v>101</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>204</v>
+        <v>101</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>206</v>
+        <v>101</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>208</v>
+        <v>101</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>210</v>
+        <v>43</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>212</v>
+        <v>43</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>214</v>
+        <v>43</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>216</v>
+        <v>43</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>218</v>
+        <v>43</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>220</v>
+        <v>43</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>222</v>
+        <v>43</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>224</v>
+        <v>43</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>226</v>
+        <v>43</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>228</v>
+        <v>43</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>230</v>
+        <v>43</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>232</v>
+        <v>43</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>234</v>
+        <v>43</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>236</v>
+        <v>43</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>238</v>
+        <v>43</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>240</v>
+        <v>43</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>242</v>
+        <v>43</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>244</v>
+        <v>43</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>246</v>
+        <v>43</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>248</v>
+        <v>43</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>250</v>
+        <v>43</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>252</v>
+        <v>43</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>254</v>
+        <v>43</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>256</v>
+        <v>43</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>258</v>
+        <v>43</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>260</v>
+        <v>43</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>262</v>
+        <v>43</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>264</v>
+        <v>43</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>266</v>
+        <v>43</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>268</v>
+        <v>43</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>270</v>
+        <v>43</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>272</v>
+        <v>43</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new prev_data set, update list/detail views, clean up JS.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/ingrowth/forms/ingrowth/ingrowth.xlsx
+++ b/odk_app/config/tables/ingrowth/forms/ingrowth/ingrowth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\ingrowth\forms\ingrowth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D1B246-DB5F-423D-A48A-8F8B7972AEAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D10C8E7-C574-4217-9FCD-2CD6843FA363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5730" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="306">
   <si>
     <t>setting_name</t>
   </si>
@@ -1075,6 +1075,9 @@
   </si>
   <si>
     <t>Stand</t>
+  </si>
+  <si>
+    <t>TreeID</t>
   </si>
 </sst>
 </file>
@@ -1684,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,24 +1739,24 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="F3" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>303</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1761,182 +1764,179 @@
         <v>30</v>
       </c>
       <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
+      <c r="A9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>46</v>
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>55</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>56</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>57</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1944,309 +1944,309 @@
         <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>46</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>68</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>69</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>70</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>73</v>
-      </c>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>46</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>74</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
         <v>75</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>76</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="A28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>46</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>79</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>80</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>81</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" t="s">
-        <v>85</v>
-      </c>
+      <c r="A32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E33" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>46</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>88</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>89</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" t="s">
         <v>90</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="A38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>46</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>94</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>95</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G39" t="s">
         <v>96</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H39" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A41" s="3"/>
       <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>39</v>
-      </c>
-      <c r="F42" t="s">
-        <v>100</v>
-      </c>
+      <c r="A42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" t="s">
-        <v>101</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="F43" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -2257,10 +2257,10 @@
         <v>101</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2271,25 +2271,39 @@
         <v>101</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>